<commit_message>
Updating repo to the current (first complete) version of the manuscript.
</commit_message>
<xml_diff>
--- a/manuscript/Supplement/Example_Datasets/example_data.xlsx
+++ b/manuscript/Supplement/Example_Datasets/example_data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal/testDataSets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Box/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal/manuscript/Supplement/Example_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257E6DE7-618C-3943-A293-076396DB2B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A441644-7521-CE43-9DD5-48B2732FC3B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36580" yWindow="10580" windowWidth="27420" windowHeight="17540" xr2:uid="{286DCE04-AB12-484B-880B-42B53AAF1A46}"/>
+    <workbookView xWindow="0" yWindow="6700" windowWidth="33600" windowHeight="20540" xr2:uid="{286DCE04-AB12-484B-880B-42B53AAF1A46}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Citations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -592,7 +592,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,7 +859,7 @@
         <v>4.9837216043291978E-3</v>
       </c>
       <c r="T4">
-        <v>124.5</v>
+        <v>100</v>
       </c>
       <c r="U4">
         <v>1255.1537590171188</v>
@@ -923,8 +923,12 @@
       <c r="S5">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="T5"/>
-      <c r="U5"/>
+      <c r="T5">
+        <v>2000</v>
+      </c>
+      <c r="U5">
+        <v>1200</v>
+      </c>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -984,8 +988,12 @@
       <c r="S6">
         <v>0.1113</v>
       </c>
-      <c r="T6"/>
-      <c r="U6"/>
+      <c r="T6">
+        <v>2000</v>
+      </c>
+      <c r="U6">
+        <v>1200</v>
+      </c>
     </row>
     <row r="7" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1045,8 +1053,12 @@
       <c r="S7">
         <v>4.3700000000000003E-2</v>
       </c>
-      <c r="T7"/>
-      <c r="U7"/>
+      <c r="T7">
+        <v>2000</v>
+      </c>
+      <c r="U7">
+        <v>1200</v>
+      </c>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1259,8 +1271,12 @@
       <c r="S11">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="T11"/>
-      <c r="U11"/>
+      <c r="T11">
+        <v>300</v>
+      </c>
+      <c r="U11">
+        <v>900</v>
+      </c>
     </row>
     <row r="12" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1308,8 +1324,12 @@
       <c r="S12">
         <v>1.23E-2</v>
       </c>
-      <c r="T12"/>
-      <c r="U12"/>
+      <c r="T12">
+        <v>300</v>
+      </c>
+      <c r="U12">
+        <v>900</v>
+      </c>
     </row>
     <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1357,8 +1377,12 @@
       <c r="S13">
         <v>1.06631828985553E-2</v>
       </c>
-      <c r="T13"/>
-      <c r="U13"/>
+      <c r="T13">
+        <v>300</v>
+      </c>
+      <c r="U13">
+        <v>900</v>
+      </c>
     </row>
     <row r="14" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1410,6 +1434,9 @@
       <c r="S14">
         <v>0.01</v>
       </c>
+      <c r="T14">
+        <v>300</v>
+      </c>
     </row>
     <row r="15" spans="1:21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1461,6 +1488,9 @@
       <c r="S15">
         <v>8.0000000000000002E-3</v>
       </c>
+      <c r="U15">
+        <v>900</v>
+      </c>
     </row>
     <row r="16" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1513,7 +1543,7 @@
         <v>0.1298</v>
       </c>
       <c r="T16">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="U16">
         <v>1050</v>
@@ -1627,7 +1657,7 @@
         <v>0.11310000000000001</v>
       </c>
       <c r="T18">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="U18">
         <v>1100</v>

</xml_diff>